<commit_message>
Add to Admin::UploadController tests, clarify code in controller
</commit_message>
<xml_diff>
--- a/spec/lib/product_import/test_data/admin_upload_template_test.xlsx
+++ b/spec/lib/product_import/test_data/admin_upload_template_test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Seller Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Short Description</t>
+  </si>
+  <si>
+    <t>Supplier Product Number</t>
   </si>
   <si>
     <t>Unit Name</t>
@@ -168,8 +171,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,13 +191,15 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,7 +551,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -562,32 +569,34 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>13.42</v>
@@ -595,13 +604,13 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>13.42</v>
@@ -609,16 +618,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
       </c>
       <c r="H4">
         <v>13.42</v>
@@ -626,13 +635,13 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>